<commit_message>
Update to present at WDI Criteria meeting
adding tree, etc.
</commit_message>
<xml_diff>
--- a/current_WDI_indicators.xlsx
+++ b/current_WDI_indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/tbenschop_worldbank_org/Documents/Documents/GitHub/WDI_GHG_emissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{FD67BC49-6828-49BE-8577-535FEC776585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA0E2C33-A9C8-46DE-B29F-CA0BAEA47270}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{FD67BC49-6828-49BE-8577-535FEC776585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDFA77C8-09D1-45DE-9FDE-5FD004E925FD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B47BD48D-1AF5-4F81-BA40-0E2B3486E8A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="90">
   <si>
     <t>Series code</t>
   </si>
@@ -274,6 +274,36 @@
   </si>
   <si>
     <t>1970-2016 (not annual)</t>
+  </si>
+  <si>
+    <t>GHG</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>N2O</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Fluorinated gases</t>
   </si>
 </sst>
 </file>
@@ -674,21 +704,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A35D4-B07D-47CD-8963-13726D4F0545}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="143" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="3" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,13 +727,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -710,13 +747,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -724,27 +767,39 @@
         <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -752,27 +807,39 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -780,27 +847,39 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -808,27 +887,39 @@
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -836,27 +927,39 @@
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -864,27 +967,39 @@
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -892,27 +1007,39 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
@@ -920,27 +1047,39 @@
         <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -948,27 +1087,39 @@
         <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -976,13 +1127,19 @@
         <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -990,27 +1147,39 @@
         <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1018,27 +1187,39 @@
         <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1046,27 +1227,39 @@
         <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1074,27 +1267,39 @@
         <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>62</v>
       </c>
@@ -1102,27 +1307,39 @@
         <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -1130,9 +1347,15 @@
         <v>29</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>